<commit_message>
Update worksheet to assist with calibration
</commit_message>
<xml_diff>
--- a/docs/20190902 m90e26_calibrate.xlsx
+++ b/docs/20190902 m90e26_calibrate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\devs\ws\z-components\devices\m90e26\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F36A580-F2A5-4199-87BF-55DBB7352CE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935B71A1-7395-489E-924D-1D683AC29C20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57975" yWindow="1575" windowWidth="18330" windowHeight="20520" xr2:uid="{FE178CC8-A0CF-4137-A708-A44CFB898DD1}"/>
+    <workbookView xWindow="15510" yWindow="360" windowWidth="21030" windowHeight="20520" activeTab="1" xr2:uid="{FE178CC8-A0CF-4137-A708-A44CFB898DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulae" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <definedName name="Cur_meaN">Formulae!$C$49</definedName>
     <definedName name="Gl">Formulae!$C$13</definedName>
     <definedName name="Ib">Formulae!$C$7</definedName>
+    <definedName name="Iratio">#REF!</definedName>
     <definedName name="Irms">Formulae!#REF!</definedName>
     <definedName name="Kn">Formulae!$C$59</definedName>
     <definedName name="KnQ">Formulae!$C$67</definedName>
@@ -49,6 +50,7 @@
     <definedName name="VlReg">Formulae!$C$43</definedName>
     <definedName name="Vn">Formulae!#REF!</definedName>
     <definedName name="Vol_mea">Formulae!$C$42</definedName>
+    <definedName name="Vratio">#REF!</definedName>
     <definedName name="Vu">Formulae!$C$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -1084,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165B2767-E119-42EF-B23D-1E7D6222F4D5}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F39AC36-C81D-9149-A2D5-F619065ABC3E}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>